<commit_message>
Write one-time import line of credit repayments script using reusable function (#720)
* Set up import line of credit repayments

* Nits

* For LOC, only fetch loans that are not closed and have origination date <= settlement date of payment
</commit_message>
<xml_diff>
--- a/services/api-server/scripts/data/icannic_repayments_2020_03_25.xlsx
+++ b/services/api-server/scripts/data/icannic_repayments_2020_03_25.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>company_id</t>
   </si>
@@ -19,16 +19,13 @@
     <t>type</t>
   </si>
   <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>payment_date</t>
-  </si>
-  <si>
     <t>deposit_date</t>
   </si>
   <si>
     <t>settlement_date</t>
+  </si>
+  <si>
+    <t>amount</t>
   </si>
   <si>
     <t>Principal Paid</t>
@@ -73,12 +70,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -91,16 +94,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -117,16 +120,16 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="4" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="4" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -146,6 +149,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -345,12 +349,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -383,10 +387,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -634,12 +638,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -954,10 +958,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1208,7 +1212,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1216,13 +1220,12 @@
   <cols>
     <col min="1" max="1" width="9.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.85156" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1719" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.3516" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.3516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85156" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="12.6719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.8516" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3516" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85156" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
@@ -1247,267 +1250,234 @@
       <c r="G1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B2" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C2" s="3">
+        <v>44018</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44018</v>
+      </c>
+      <c r="E2" s="4">
         <v>4079.25</v>
       </c>
-      <c r="D2" s="4">
-        <v>44018</v>
-      </c>
-      <c r="E2" s="4">
-        <v>44018</v>
-      </c>
       <c r="F2" s="4">
-        <v>44018</v>
-      </c>
-      <c r="G2" s="3">
         <v>0</v>
       </c>
-      <c r="H2" s="5">
+      <c r="G2" s="5">
         <v>4079.25</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C3" s="3">
+        <v>44046</v>
+      </c>
+      <c r="D3" s="3">
+        <v>44048</v>
+      </c>
+      <c r="E3" s="4">
         <v>130000</v>
       </c>
-      <c r="D3" s="4">
-        <v>44046</v>
-      </c>
-      <c r="E3" s="4">
-        <v>44046</v>
-      </c>
-      <c r="F3" s="4">
-        <v>44048</v>
+      <c r="F3" s="5">
+        <v>123978.25</v>
       </c>
       <c r="G3" s="5">
-        <v>123978.25</v>
-      </c>
-      <c r="H3" s="5">
         <v>6021.75</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1">
       <c r="A4" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B4" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C4" s="3">
+        <v>44082</v>
+      </c>
+      <c r="D4" s="3">
+        <v>44082</v>
+      </c>
+      <c r="E4" s="4">
         <v>4632.07</v>
       </c>
-      <c r="D4" s="4">
-        <v>44082</v>
-      </c>
-      <c r="E4" s="4">
-        <v>44082</v>
-      </c>
       <c r="F4" s="4">
-        <v>44082</v>
-      </c>
-      <c r="G4" s="3">
         <v>0</v>
       </c>
-      <c r="H4" s="5">
+      <c r="G4" s="5">
         <v>4632.07</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B5" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C5" s="3">
+        <v>44109</v>
+      </c>
+      <c r="D5" s="3">
+        <v>44109</v>
+      </c>
+      <c r="E5" s="4">
         <v>5072.1</v>
       </c>
-      <c r="D5" s="4">
-        <v>44109</v>
-      </c>
-      <c r="E5" s="4">
-        <v>44109</v>
-      </c>
       <c r="F5" s="4">
-        <v>44109</v>
-      </c>
-      <c r="G5" s="3">
         <v>0</v>
       </c>
-      <c r="H5" s="5">
+      <c r="G5" s="5">
         <v>5072.1</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B6" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C6" s="3">
+        <v>44140</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44140</v>
+      </c>
+      <c r="E6" s="4">
         <v>5787.17</v>
       </c>
-      <c r="D6" s="4">
-        <v>44140</v>
-      </c>
-      <c r="E6" s="4">
-        <v>44140</v>
-      </c>
       <c r="F6" s="4">
-        <v>44140</v>
-      </c>
-      <c r="G6" s="3">
         <v>0</v>
       </c>
-      <c r="H6" s="5">
+      <c r="G6" s="5">
         <v>5787.17</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B7" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C7" s="3">
+        <v>44169</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44169</v>
+      </c>
+      <c r="E7" s="4">
         <v>6332.1</v>
       </c>
-      <c r="D7" s="4">
-        <v>44169</v>
-      </c>
-      <c r="E7" s="4">
-        <v>44169</v>
-      </c>
       <c r="F7" s="4">
-        <v>44169</v>
-      </c>
-      <c r="G7" s="3">
         <v>0</v>
       </c>
-      <c r="H7" s="5">
+      <c r="G7" s="5">
         <v>6332.1</v>
       </c>
     </row>
     <row r="8" ht="14.25" customHeight="1">
       <c r="A8" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B8" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C8" s="3">
+        <v>44182</v>
+      </c>
+      <c r="D8" s="3">
+        <v>44186</v>
+      </c>
+      <c r="E8" s="4">
         <v>50000</v>
       </c>
-      <c r="D8" s="4">
-        <v>44182</v>
-      </c>
-      <c r="E8" s="4">
-        <v>44182</v>
-      </c>
-      <c r="F8" s="4">
-        <v>44186</v>
-      </c>
-      <c r="G8" s="5">
+      <c r="F8" s="5">
         <v>50000</v>
       </c>
-      <c r="H8" s="3">
+      <c r="G8" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="9" ht="14.25" customHeight="1">
       <c r="A9" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C9" s="3">
+        <v>44201</v>
+      </c>
+      <c r="D9" s="3">
+        <v>44201</v>
+      </c>
+      <c r="E9" s="4">
         <v>6018.17</v>
       </c>
-      <c r="D9" s="4">
-        <v>44201</v>
-      </c>
-      <c r="E9" s="4">
-        <v>44201</v>
-      </c>
       <c r="F9" s="4">
-        <v>44201</v>
-      </c>
-      <c r="G9" s="3">
         <v>0</v>
       </c>
-      <c r="H9" s="5">
+      <c r="G9" s="5">
         <v>6018.17</v>
       </c>
     </row>
     <row r="10" ht="14.25" customHeight="1">
       <c r="A10" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B10" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C10" s="3">
+        <v>44232</v>
+      </c>
+      <c r="D10" s="3">
+        <v>44232</v>
+      </c>
+      <c r="E10" s="4">
         <v>4915.67</v>
       </c>
-      <c r="D10" s="4">
-        <v>44232</v>
-      </c>
-      <c r="E10" s="4">
-        <v>44232</v>
-      </c>
       <c r="F10" s="4">
-        <v>44232</v>
-      </c>
-      <c r="G10" s="3">
         <v>0</v>
       </c>
-      <c r="H10" s="5">
+      <c r="G10" s="5">
         <v>4915.67</v>
       </c>
     </row>
     <row r="11" ht="14.25" customHeight="1">
       <c r="A11" t="s" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="B11" t="s" s="2">
-        <v>9</v>
-      </c>
       <c r="C11" s="3">
+        <v>44260</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44260</v>
+      </c>
+      <c r="E11" s="4">
         <v>4439.96</v>
       </c>
-      <c r="D11" s="4">
-        <v>44260</v>
-      </c>
-      <c r="E11" s="4">
-        <v>44260</v>
-      </c>
       <c r="F11" s="4">
-        <v>44260</v>
-      </c>
-      <c r="G11" s="3">
         <v>0</v>
       </c>
-      <c r="H11" s="5">
+      <c r="G11" s="5">
         <v>4439.96</v>
       </c>
     </row>

</xml_diff>